<commit_message>
Add Ceftazidime-Avibactam and filter available products
</commit_message>
<xml_diff>
--- a/docs/assets/antibiogram.xlsx
+++ b/docs/assets/antibiogram.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -288,6 +288,21 @@
   </si>
   <si>
     <t>e.g. Mycoplasma sp.</t>
+  </si>
+  <si>
+    <t>ESBL</t>
+  </si>
+  <si>
+    <t>CPE</t>
+  </si>
+  <si>
+    <t>VRE</t>
+  </si>
+  <si>
+    <t>Ceftazidime/Avibactam</t>
+  </si>
+  <si>
+    <t>Cephalosporins with beta-lactamase inhibitors</t>
   </si>
 </sst>
 </file>
@@ -381,7 +396,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +508,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,7 +672,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -746,6 +767,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -755,9 +899,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,15 +917,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -803,15 +935,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,107 +944,17 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -929,127 +962,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1124,6 +1037,129 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1150,59 +1186,95 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AM13" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:AM13"/>
-  <tableColumns count="39">
-    <tableColumn id="1" name="Group" dataDxfId="38"/>
-    <tableColumn id="2" name="Name" dataDxfId="37"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="36"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="35"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="34"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="33"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="32"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="31"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="30"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="29"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="28"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="27"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="26"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="25"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="24"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="23"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="22"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="21"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="20"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="19"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="18"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="17"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="16"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="15"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="14"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="13"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="12"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="11"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="10"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="9"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="8"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="7"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="6"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="5"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="4"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="3"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="2"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="1"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AN16" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="A1:AN16"/>
+  <tableColumns count="40">
+    <tableColumn id="1" name="Group" dataDxfId="43"/>
+    <tableColumn id="2" name="Name" dataDxfId="42"/>
+    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="41"/>
+    <tableColumn id="4" name="Naficillin" dataDxfId="40"/>
+    <tableColumn id="5" name="Oxacillin" dataDxfId="39"/>
+    <tableColumn id="6" name="Flucloxacillin" dataDxfId="38"/>
+    <tableColumn id="7" name="Ampicillin" dataDxfId="37"/>
+    <tableColumn id="8" name="Amoxicillin" dataDxfId="36"/>
+    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="35"/>
+    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="34"/>
+    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="33"/>
+    <tableColumn id="12" name="Cefazolin" dataDxfId="32"/>
+    <tableColumn id="13" name="Cefalexin" dataDxfId="31"/>
+    <tableColumn id="14" name="Cefuroxime" dataDxfId="30"/>
+    <tableColumn id="15" name="Cephotetan" dataDxfId="29"/>
+    <tableColumn id="16" name="Cefoxitin" dataDxfId="28"/>
+    <tableColumn id="17" name="Cefotaxime" dataDxfId="27"/>
+    <tableColumn id="18" name="Ceftriaxone" dataDxfId="26"/>
+    <tableColumn id="19" name="Ceftazidime" dataDxfId="25"/>
+    <tableColumn id="20" name="Cefepime" dataDxfId="24"/>
+    <tableColumn id="21" name="Ceftaroline" dataDxfId="23"/>
+    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="0"/>
+    <tableColumn id="22" name="Ertapenem" dataDxfId="22"/>
+    <tableColumn id="23" name="Imipenem" dataDxfId="21"/>
+    <tableColumn id="24" name="Meropenem" dataDxfId="20"/>
+    <tableColumn id="25" name="Aztreonam" dataDxfId="19"/>
+    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="18"/>
+    <tableColumn id="27" name="Levofloxacin" dataDxfId="17"/>
+    <tableColumn id="28" name="Moxifloxacin" dataDxfId="16"/>
+    <tableColumn id="29" name="Gentamicin" dataDxfId="15"/>
+    <tableColumn id="30" name="Tobramycin" dataDxfId="14"/>
+    <tableColumn id="31" name="Amikacin" dataDxfId="13"/>
+    <tableColumn id="32" name="Azithromycin" dataDxfId="12"/>
+    <tableColumn id="33" name="Clindamycin" dataDxfId="11"/>
+    <tableColumn id="34" name="Doxycycline" dataDxfId="10"/>
+    <tableColumn id="35" name="Vancomycin" dataDxfId="9"/>
+    <tableColumn id="36" name="Daptomycin" dataDxfId="8"/>
+    <tableColumn id="37" name="Linezolid" dataDxfId="7"/>
+    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="6"/>
+    <tableColumn id="39" name="Metronidazole" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:B38" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:B38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:B39" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:B39">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Amikacin"/>
+        <filter val="Amoxicillin"/>
+        <filter val="Amoxicillin-Clavulanic Acid"/>
+        <filter val="Azithromycin"/>
+        <filter val="Aztreonam"/>
+        <filter val="Benzylpenicillin"/>
+        <filter val="Cefalexin"/>
+        <filter val="Cefazolin"/>
+        <filter val="Cefotaxime"/>
+        <filter val="Ceftaroline"/>
+        <filter val="Ceftazidime"/>
+        <filter val="Ceftazidime/Avibactam"/>
+        <filter val="Ceftriaxone"/>
+        <filter val="Cefuroxime"/>
+        <filter val="Ciprofloxacin"/>
+        <filter val="Clindamycin"/>
+        <filter val="Daptomycin"/>
+        <filter val="Doxycycline"/>
+        <filter val="Ertapenem"/>
+        <filter val="Flucloxacillin"/>
+        <filter val="Gentamicin"/>
+        <filter val="Levofloxacin"/>
+        <filter val="Linezolid"/>
+        <filter val="Meropenem"/>
+        <filter val="Metronidazole"/>
+        <filter val="Moxifloxacin"/>
+        <filter val="Piperacillin-Tazobactam"/>
+        <filter val="Tobramycin"/>
+        <filter val="Trimethoprim/Sulfamethoxazole"/>
+        <filter val="Vancomycin"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Drug Name" dataDxfId="42"/>
-    <tableColumn id="2" name="Drug Class" dataDxfId="41"/>
+    <tableColumn id="1" name="Drug Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Drug Class" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1463,7 +1535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1474,12 +1546,12 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AM13"/>
+  <dimension ref="A1:AN16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="10320" ySplit="7875" topLeftCell="A25" activePane="bottomLeft"/>
-      <selection activeCell="C21" sqref="C21"/>
-      <selection pane="topRight"/>
+      <pane xSplit="10320" ySplit="7875" topLeftCell="R25" activePane="topRight"/>
+      <selection activeCell="C20" sqref="C20"/>
+      <selection pane="topRight" activeCell="U18" sqref="U18"/>
       <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
       <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
@@ -1505,7 +1577,8 @@
     <col min="18" max="18" width="12.625" style="33" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.75" style="33" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23" style="33" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.375" style="33" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.375" style="33" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.25" style="33" bestFit="1" customWidth="1"/>
@@ -1525,7 +1598,7 @@
     <col min="40" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>78</v>
       </c>
@@ -1590,61 +1663,64 @@
         <v>72</v>
       </c>
       <c r="V1" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="W1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="33" t="s">
+      <c r="AE1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AF1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AG1" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AI1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="AM1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -1654,9 +1730,6 @@
       <c r="U2" s="33">
         <v>1</v>
       </c>
-      <c r="AG2" s="33">
-        <v>1</v>
-      </c>
       <c r="AH2" s="33">
         <v>1</v>
       </c>
@@ -1672,8 +1745,11 @@
       <c r="AL2" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM2" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
@@ -1725,16 +1801,13 @@
       <c r="U3" s="33">
         <v>1</v>
       </c>
-      <c r="V3" s="33">
-        <v>1</v>
-      </c>
       <c r="W3" s="33">
         <v>1</v>
       </c>
       <c r="X3" s="33">
         <v>1</v>
       </c>
-      <c r="Z3" s="33">
+      <c r="Y3" s="33">
         <v>1</v>
       </c>
       <c r="AA3" s="33">
@@ -1743,7 +1816,7 @@
       <c r="AB3" s="33">
         <v>1</v>
       </c>
-      <c r="AF3" s="33">
+      <c r="AC3" s="33">
         <v>1</v>
       </c>
       <c r="AG3" s="33">
@@ -1764,8 +1837,11 @@
       <c r="AL3" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM3" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
@@ -1838,13 +1914,13 @@
       <c r="X4" s="33">
         <v>1</v>
       </c>
-      <c r="AA4" s="33">
+      <c r="Y4" s="33">
         <v>1</v>
       </c>
       <c r="AB4" s="33">
         <v>1</v>
       </c>
-      <c r="AF4" s="33">
+      <c r="AC4" s="33">
         <v>1</v>
       </c>
       <c r="AG4" s="33">
@@ -1865,8 +1941,11 @@
       <c r="AL4" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM4" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>80</v>
       </c>
@@ -1948,14 +2027,17 @@
       <c r="AE5" s="33">
         <v>1</v>
       </c>
-      <c r="AH5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AF5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>80</v>
       </c>
@@ -2037,11 +2119,14 @@
       <c r="AE6" s="33">
         <v>1</v>
       </c>
-      <c r="AL6" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AF6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>80</v>
       </c>
@@ -2117,11 +2202,14 @@
       <c r="AE7" s="33">
         <v>1</v>
       </c>
-      <c r="AL7" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AF7" s="33">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>80</v>
       </c>
@@ -2137,7 +2225,7 @@
       <c r="T8" s="33">
         <v>1</v>
       </c>
-      <c r="W8" s="33">
+      <c r="V8" s="33">
         <v>1</v>
       </c>
       <c r="X8" s="33">
@@ -2152,7 +2240,7 @@
       <c r="AA8" s="33">
         <v>1</v>
       </c>
-      <c r="AC8" s="33">
+      <c r="AB8" s="33">
         <v>1</v>
       </c>
       <c r="AD8" s="33">
@@ -2161,12 +2249,15 @@
       <c r="AE8" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AF8" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="93" t="s">
         <v>5</v>
       </c>
       <c r="K9" s="33">
@@ -2184,9 +2275,6 @@
       <c r="U9" s="33">
         <v>1</v>
       </c>
-      <c r="V9" s="33">
-        <v>1</v>
-      </c>
       <c r="W9" s="33">
         <v>1</v>
       </c>
@@ -2214,7 +2302,7 @@
       <c r="AE9" s="33">
         <v>1</v>
       </c>
-      <c r="AJ9" s="33">
+      <c r="AF9" s="33">
         <v>1</v>
       </c>
       <c r="AK9" s="33">
@@ -2223,8 +2311,11 @@
       <c r="AL9" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM9" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>81</v>
       </c>
@@ -2237,9 +2328,6 @@
       <c r="T10" s="33">
         <v>1</v>
       </c>
-      <c r="V10" s="33">
-        <v>1</v>
-      </c>
       <c r="W10" s="33">
         <v>1</v>
       </c>
@@ -2258,8 +2346,11 @@
       <c r="AB10" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AC10" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
@@ -2284,9 +2375,6 @@
       <c r="T11" s="33">
         <v>1</v>
       </c>
-      <c r="V11" s="33">
-        <v>1</v>
-      </c>
       <c r="W11" s="33">
         <v>1</v>
       </c>
@@ -2305,17 +2393,20 @@
       <c r="AB11" s="33">
         <v>1</v>
       </c>
-      <c r="AF11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AC11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
@@ -2337,43 +2428,61 @@
       <c r="P12" s="33">
         <v>1</v>
       </c>
-      <c r="V12" s="33">
-        <v>1</v>
-      </c>
       <c r="W12" s="33">
         <v>1</v>
       </c>
       <c r="X12" s="33">
         <v>1</v>
       </c>
-      <c r="AB12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="Y12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="AA13" s="33">
-        <v>1</v>
-      </c>
       <c r="AB13" s="33">
         <v>1</v>
       </c>
-      <c r="AF13" s="33">
-        <v>1</v>
-      </c>
-      <c r="AH13" s="33">
-        <v>1</v>
+      <c r="AC13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="V14" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2389,10 +2498,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2418,16 +2527,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="94" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="94" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="31" t="s">
@@ -2442,8 +2551,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="94" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="31" t="s">
@@ -2466,8 +2575,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="94" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="31" t="s">
@@ -2506,16 +2615,16 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="94" t="s">
         <v>66</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="94" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="31" t="s">
@@ -2546,7 +2655,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>9</v>
       </c>
@@ -2563,24 +2672,24 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>42</v>
+      <c r="A21" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="96" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>63</v>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
+        <v>62</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>42</v>
@@ -2588,23 +2697,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B25" s="31" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>38</v>
@@ -2612,23 +2721,23 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>56</v>
+      <c r="A28" s="95" t="s">
+        <v>14</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>35</v>
@@ -2636,7 +2745,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>35</v>
@@ -2644,65 +2753,73 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B39" s="31" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2749,23 +2866,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="88"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="35" t="s">
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="61" t="s">
+      <c r="K1" s="77"/>
+      <c r="L1" s="58" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -2806,7 +2923,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="62"/>
+      <c r="L2" s="59"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -2836,11 +2953,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="38" t="str">
+      <c r="C4" s="78" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2857,12 +2974,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="38" t="str">
+      <c r="D5" s="78" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2879,14 +2996,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="41" t="str">
+      <c r="C6" s="81" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="83"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -2899,14 +3016,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="41" t="str">
+      <c r="C7" s="81" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="43"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="83"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -2922,21 +3039,21 @@
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="41" t="str">
+      <c r="C8" s="81" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="43"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="41" t="str">
+      <c r="I8" s="81" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="56"/>
-      <c r="K8" s="43"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="83"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
@@ -2944,14 +3061,14 @@
       <c r="A9" s="37"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="41" t="str">
+      <c r="D9" s="81" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="43"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="83"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -2963,18 +3080,18 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="57" t="str">
+      <c r="C10" s="91" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="43"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="83"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
@@ -2983,14 +3100,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="44" t="str">
+      <c r="C11" s="52" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -3004,14 +3121,14 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="44" t="str">
+      <c r="C12" s="52" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="46"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -3025,22 +3142,22 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="59" t="str">
+      <c r="C13" s="66" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="60"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="68"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="59" t="str">
+      <c r="K13" s="66" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="60"/>
+      <c r="L13" s="68"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3048,40 +3165,40 @@
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="70" t="str">
-        <f>'Drug Information'!$A21</f>
+      <c r="C14" s="69" t="str">
+        <f>'Drug Information'!$A22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="72"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="70" t="str">
-        <f>'Drug Information'!$A21</f>
+      <c r="I14" s="69" t="str">
+        <f>'Drug Information'!$A22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="72"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="71"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="70" t="str">
-        <f>'Drug Information'!$A23</f>
+      <c r="C15" s="69" t="str">
+        <f>'Drug Information'!$A24</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="72"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="71"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3091,15 +3208,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="73" t="s">
+      <c r="E16" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="75"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="74"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
@@ -3109,64 +3226,64 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="12" t="str">
-        <f>'Drug Information'!$A25</f>
+        <f>'Drug Information'!$A26</f>
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="79" t="str">
-        <f>'Drug Information'!$A25</f>
+      <c r="E17" s="38" t="str">
+        <f>'Drug Information'!$A26</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="81"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="37"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="79" t="str">
-        <f>'Drug Information'!$A26</f>
+      <c r="C18" s="38" t="str">
+        <f>'Drug Information'!$A27</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="83"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
-        <f>'Drug Information'!$A26</f>
+        <f>'Drug Information'!$A27</f>
         <v>Levofloxacin</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="53" t="str">
-        <f>'Drug Information'!$A27</f>
+      <c r="C19" s="43" t="str">
+        <f>'Drug Information'!$A28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="55"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="53" t="str">
-        <f>'Drug Information'!$A27</f>
+      <c r="I19" s="43" t="str">
+        <f>'Drug Information'!$A28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="55"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3175,14 +3292,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="86" t="str">
-        <f>'Drug Information'!$A30</f>
+      <c r="E20" s="48" t="str">
+        <f>'Drug Information'!$A31</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="89"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -3192,12 +3309,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="63" t="str">
-        <f>'Drug Information'!$A32</f>
+      <c r="B21" s="60" t="str">
+        <f>'Drug Information'!$A33</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3206,7 +3323,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="13" t="str">
-        <f>'Drug Information'!$A32</f>
+        <f>'Drug Information'!$A33</f>
         <v>Clindamycin</v>
       </c>
       <c r="M21" s="14"/>
@@ -3216,11 +3333,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="84" t="str">
-        <f>'Drug Information'!$A31</f>
+      <c r="C22" s="46" t="str">
+        <f>'Drug Information'!$A32</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="85"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3228,12 +3345,12 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="15" t="str">
-        <f>'Drug Information'!$A31</f>
+        <f>'Drug Information'!$A32</f>
         <v>Azithromycin</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="16" t="str">
-        <f>'Drug Information'!$A31</f>
+        <f>'Drug Information'!$A32</f>
         <v>Azithromycin</v>
       </c>
     </row>
@@ -3241,25 +3358,25 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="90" t="str">
-        <f>'Drug Information'!$A33</f>
+      <c r="B23" s="55" t="str">
+        <f>'Drug Information'!$A34</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="92"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="17" t="str">
-        <f>'Drug Information'!$A33</f>
+        <f>'Drug Information'!$A34</f>
         <v>Doxycycline</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="17" t="str">
-        <f>'Drug Information'!$A33</f>
+        <f>'Drug Information'!$A34</f>
         <v>Doxycycline</v>
       </c>
     </row>
@@ -3267,12 +3384,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="66" t="str">
-        <f>'Drug Information'!$A34</f>
+      <c r="B24" s="63" t="str">
+        <f>'Drug Information'!$A35</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3287,15 +3404,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="76" t="str">
-        <f>'Drug Information'!$A37</f>
+      <c r="B25" s="34" t="str">
+        <f>'Drug Information'!$A38</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="78"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -3322,49 +3439,30 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="20" t="str">
-        <f>'Drug Information'!$A38</f>
+        <f>'Drug Information'!$A39</f>
         <v>Metronidazole</v>
       </c>
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -3381,6 +3479,25 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add "Include" column to Excel file and inclusion handling to code
</commit_message>
<xml_diff>
--- a/docs/assets/antibiogram.xlsx
+++ b/docs/assets/antibiogram.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="91">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>Cephalosporins with beta-lactamase inhibitors</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -767,31 +773,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -803,40 +851,19 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -863,15 +890,9 @@
     <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -890,71 +911,56 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -962,7 +968,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="48">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1037,6 +1043,27 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1186,95 +1213,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AN16" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
-  <autoFilter ref="A1:AN16"/>
-  <tableColumns count="40">
-    <tableColumn id="1" name="Group" dataDxfId="43"/>
-    <tableColumn id="2" name="Name" dataDxfId="42"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="41"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="40"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="39"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="38"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="37"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="36"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="35"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="34"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="33"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="32"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="31"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="30"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="29"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="28"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="27"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="26"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="25"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="24"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="23"/>
-    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="0"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="22"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="21"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="20"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="19"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="18"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="17"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="16"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="15"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="14"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="13"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="12"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="11"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="10"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="9"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="8"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="7"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="6"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AO16" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="A1:AO16"/>
+  <tableColumns count="41">
+    <tableColumn id="1" name="Group" dataDxfId="45"/>
+    <tableColumn id="2" name="Name" dataDxfId="44"/>
+    <tableColumn id="41" name="Include" dataDxfId="0"/>
+    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="43"/>
+    <tableColumn id="4" name="Naficillin" dataDxfId="42"/>
+    <tableColumn id="5" name="Oxacillin" dataDxfId="41"/>
+    <tableColumn id="6" name="Flucloxacillin" dataDxfId="40"/>
+    <tableColumn id="7" name="Ampicillin" dataDxfId="39"/>
+    <tableColumn id="8" name="Amoxicillin" dataDxfId="38"/>
+    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="37"/>
+    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="36"/>
+    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="35"/>
+    <tableColumn id="12" name="Cefazolin" dataDxfId="34"/>
+    <tableColumn id="13" name="Cefalexin" dataDxfId="33"/>
+    <tableColumn id="14" name="Cefuroxime" dataDxfId="32"/>
+    <tableColumn id="15" name="Cephotetan" dataDxfId="31"/>
+    <tableColumn id="16" name="Cefoxitin" dataDxfId="30"/>
+    <tableColumn id="17" name="Cefotaxime" dataDxfId="29"/>
+    <tableColumn id="18" name="Ceftriaxone" dataDxfId="28"/>
+    <tableColumn id="19" name="Ceftazidime" dataDxfId="27"/>
+    <tableColumn id="20" name="Cefepime" dataDxfId="26"/>
+    <tableColumn id="21" name="Ceftaroline" dataDxfId="25"/>
+    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="24"/>
+    <tableColumn id="22" name="Ertapenem" dataDxfId="23"/>
+    <tableColumn id="23" name="Imipenem" dataDxfId="22"/>
+    <tableColumn id="24" name="Meropenem" dataDxfId="21"/>
+    <tableColumn id="25" name="Aztreonam" dataDxfId="20"/>
+    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="19"/>
+    <tableColumn id="27" name="Levofloxacin" dataDxfId="18"/>
+    <tableColumn id="28" name="Moxifloxacin" dataDxfId="17"/>
+    <tableColumn id="29" name="Gentamicin" dataDxfId="16"/>
+    <tableColumn id="30" name="Tobramycin" dataDxfId="15"/>
+    <tableColumn id="31" name="Amikacin" dataDxfId="14"/>
+    <tableColumn id="32" name="Azithromycin" dataDxfId="13"/>
+    <tableColumn id="33" name="Clindamycin" dataDxfId="12"/>
+    <tableColumn id="34" name="Doxycycline" dataDxfId="11"/>
+    <tableColumn id="35" name="Vancomycin" dataDxfId="10"/>
+    <tableColumn id="36" name="Daptomycin" dataDxfId="9"/>
+    <tableColumn id="37" name="Linezolid" dataDxfId="8"/>
+    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="7"/>
+    <tableColumn id="39" name="Metronidazole" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:B39" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:B39">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Amikacin"/>
-        <filter val="Amoxicillin"/>
-        <filter val="Amoxicillin-Clavulanic Acid"/>
-        <filter val="Azithromycin"/>
-        <filter val="Aztreonam"/>
-        <filter val="Benzylpenicillin"/>
-        <filter val="Cefalexin"/>
-        <filter val="Cefazolin"/>
-        <filter val="Cefotaxime"/>
-        <filter val="Ceftaroline"/>
-        <filter val="Ceftazidime"/>
-        <filter val="Ceftazidime/Avibactam"/>
-        <filter val="Ceftriaxone"/>
-        <filter val="Cefuroxime"/>
-        <filter val="Ciprofloxacin"/>
-        <filter val="Clindamycin"/>
-        <filter val="Daptomycin"/>
-        <filter val="Doxycycline"/>
-        <filter val="Ertapenem"/>
-        <filter val="Flucloxacillin"/>
-        <filter val="Gentamicin"/>
-        <filter val="Levofloxacin"/>
-        <filter val="Linezolid"/>
-        <filter val="Meropenem"/>
-        <filter val="Metronidazole"/>
-        <filter val="Moxifloxacin"/>
-        <filter val="Piperacillin-Tazobactam"/>
-        <filter val="Tobramycin"/>
-        <filter val="Trimethoprim/Sulfamethoxazole"/>
-        <filter val="Vancomycin"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Drug Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Drug Class" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:C39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:C39"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Drug Name" dataDxfId="3"/>
+    <tableColumn id="2" name="Drug Class" dataDxfId="2"/>
+    <tableColumn id="3" name="Include" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1535,7 +1529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,13 +1540,13 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AN16"/>
+  <dimension ref="A1:AO16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="10320" ySplit="7875" topLeftCell="R25" activePane="topRight"/>
-      <selection activeCell="C20" sqref="C20"/>
+      <pane xSplit="10320" ySplit="7875" topLeftCell="A25"/>
+      <selection activeCell="D21" sqref="D21"/>
       <selection pane="topRight" activeCell="U18" sqref="U18"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
       <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1560,45 +1554,46 @@
   <cols>
     <col min="1" max="1" width="18.375" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.125" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.875" style="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23" style="33" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14" style="33" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13" style="33" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13" style="33" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="13.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="31.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9" style="33"/>
+    <col min="3" max="3" width="18.75" style="33" customWidth="1"/>
+    <col min="4" max="4" width="16.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23" style="33" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" style="33" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" style="33" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13" style="33" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="13.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>78</v>
       </c>
@@ -1606,131 +1601,134 @@
         <v>79</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="S1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="33" t="s">
+      <c r="AE1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AF1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AG1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AM1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="AN1" s="33" t="s">
+      <c r="AO1" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="33">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="33">
+      <c r="C2" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="33">
         <v>1</v>
       </c>
       <c r="AI2" s="33">
@@ -1748,16 +1746,19 @@
       <c r="AM2" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AN2" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="33">
-        <v>1</v>
+      <c r="C3" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="E3" s="33">
         <v>1</v>
@@ -1765,7 +1766,7 @@
       <c r="F3" s="33">
         <v>1</v>
       </c>
-      <c r="I3" s="33">
+      <c r="G3" s="33">
         <v>1</v>
       </c>
       <c r="J3" s="33">
@@ -1795,13 +1796,13 @@
       <c r="R3" s="33">
         <v>1</v>
       </c>
-      <c r="T3" s="33">
+      <c r="S3" s="33">
         <v>1</v>
       </c>
       <c r="U3" s="33">
         <v>1</v>
       </c>
-      <c r="W3" s="33">
+      <c r="V3" s="33">
         <v>1</v>
       </c>
       <c r="X3" s="33">
@@ -1810,7 +1811,7 @@
       <c r="Y3" s="33">
         <v>1</v>
       </c>
-      <c r="AA3" s="33">
+      <c r="Z3" s="33">
         <v>1</v>
       </c>
       <c r="AB3" s="33">
@@ -1819,7 +1820,7 @@
       <c r="AC3" s="33">
         <v>1</v>
       </c>
-      <c r="AG3" s="33">
+      <c r="AD3" s="33">
         <v>1</v>
       </c>
       <c r="AH3" s="33">
@@ -1840,16 +1841,19 @@
       <c r="AM3" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AN3" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="33">
-        <v>1</v>
+      <c r="C4" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="D4" s="33">
         <v>1</v>
@@ -1917,13 +1921,13 @@
       <c r="Y4" s="33">
         <v>1</v>
       </c>
-      <c r="AB4" s="33">
+      <c r="Z4" s="33">
         <v>1</v>
       </c>
       <c r="AC4" s="33">
         <v>1</v>
       </c>
-      <c r="AG4" s="33">
+      <c r="AD4" s="33">
         <v>1</v>
       </c>
       <c r="AH4" s="33">
@@ -1944,16 +1948,19 @@
       <c r="AM4" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AN4" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="33">
-        <v>1</v>
+      <c r="C5" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="H5" s="33">
         <v>1</v>
@@ -2030,22 +2037,25 @@
       <c r="AF5" s="33">
         <v>1</v>
       </c>
-      <c r="AI5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AG5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="33">
-        <v>1</v>
+      <c r="C6" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="H6" s="33">
         <v>1</v>
@@ -2122,19 +2132,22 @@
       <c r="AF6" s="33">
         <v>1</v>
       </c>
-      <c r="AM6" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AG6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="33">
-        <v>1</v>
+      <c r="C7" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="J7" s="33">
         <v>1</v>
@@ -2205,30 +2218,33 @@
       <c r="AF7" s="33">
         <v>1</v>
       </c>
-      <c r="AM7" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AG7" s="33">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="33">
-        <v>1</v>
-      </c>
-      <c r="S8" s="33">
+      <c r="C8" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="33">
         <v>1</v>
       </c>
       <c r="T8" s="33">
         <v>1</v>
       </c>
-      <c r="V8" s="33">
-        <v>1</v>
-      </c>
-      <c r="X8" s="33">
+      <c r="U8" s="33">
+        <v>1</v>
+      </c>
+      <c r="W8" s="33">
         <v>1</v>
       </c>
       <c r="Y8" s="33">
@@ -2243,7 +2259,7 @@
       <c r="AB8" s="33">
         <v>1</v>
       </c>
-      <c r="AD8" s="33">
+      <c r="AC8" s="33">
         <v>1</v>
       </c>
       <c r="AE8" s="33">
@@ -2252,30 +2268,33 @@
       <c r="AF8" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AG8" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="33">
+      <c r="C9" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="33">
         <v>1</v>
       </c>
       <c r="R9" s="33">
         <v>1</v>
       </c>
-      <c r="T9" s="33">
+      <c r="S9" s="33">
         <v>1</v>
       </c>
       <c r="U9" s="33">
         <v>1</v>
       </c>
-      <c r="W9" s="33">
+      <c r="V9" s="33">
         <v>1</v>
       </c>
       <c r="X9" s="33">
@@ -2305,7 +2324,7 @@
       <c r="AF9" s="33">
         <v>1</v>
       </c>
-      <c r="AK9" s="33">
+      <c r="AG9" s="33">
         <v>1</v>
       </c>
       <c r="AL9" s="33">
@@ -2314,21 +2333,24 @@
       <c r="AM9" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AN9" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="33">
-        <v>1</v>
-      </c>
-      <c r="T10" s="33">
-        <v>1</v>
-      </c>
-      <c r="W10" s="33">
+      <c r="C10" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="S10" s="33">
+        <v>1</v>
+      </c>
+      <c r="U10" s="33">
         <v>1</v>
       </c>
       <c r="X10" s="33">
@@ -2349,33 +2371,36 @@
       <c r="AC10" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AD10" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="33">
-        <v>1</v>
+      <c r="C11" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="H11" s="33">
         <v>1</v>
       </c>
-      <c r="K11" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="33">
+      <c r="I11" s="33">
+        <v>1</v>
+      </c>
+      <c r="L11" s="33">
         <v>1</v>
       </c>
       <c r="R11" s="33">
         <v>1</v>
       </c>
-      <c r="T11" s="33">
-        <v>1</v>
-      </c>
-      <c r="W11" s="33">
+      <c r="S11" s="33">
+        <v>1</v>
+      </c>
+      <c r="U11" s="33">
         <v>1</v>
       </c>
       <c r="X11" s="33">
@@ -2396,25 +2421,28 @@
       <c r="AC11" s="33">
         <v>1</v>
       </c>
-      <c r="AG11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AD11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="33">
-        <v>1</v>
+      <c r="C12" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="J12" s="33">
         <v>1</v>
@@ -2422,13 +2450,13 @@
       <c r="K12" s="33">
         <v>1</v>
       </c>
-      <c r="O12" s="33">
+      <c r="L12" s="33">
         <v>1</v>
       </c>
       <c r="P12" s="33">
         <v>1</v>
       </c>
-      <c r="W12" s="33">
+      <c r="Q12" s="33">
         <v>1</v>
       </c>
       <c r="X12" s="33">
@@ -2437,52 +2465,67 @@
       <c r="Y12" s="33">
         <v>1</v>
       </c>
-      <c r="AC12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AN12" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="Z12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="AB13" s="33">
-        <v>1</v>
+      <c r="C13" s="33" t="s">
+        <v>90</v>
       </c>
       <c r="AC13" s="33">
         <v>1</v>
       </c>
-      <c r="AG13" s="33">
-        <v>1</v>
-      </c>
-      <c r="AI13" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AD13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="V14" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C14" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="W14" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C15" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>86</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2498,329 +2541,431 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.875" style="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.875" style="32" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="32"/>
+    <col min="3" max="3" width="17.875" style="32" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="C2" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="C3" s="37"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="C5" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="37"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="94" t="s">
+      <c r="C8" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="37"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+      <c r="C13" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
         <v>66</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="94" t="s">
+      <c r="C14" s="37"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="37"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="96" t="s">
+      <c r="C20" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="37" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="94" t="s">
+      <c r="C22" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="37"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="95" t="s">
+      <c r="C24" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="95" t="s">
+      <c r="C27" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>73</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>24</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2866,23 +3011,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="84" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="76" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="77"/>
-      <c r="L1" s="58" t="s">
+      <c r="K1" s="40"/>
+      <c r="L1" s="65" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -2923,7 +3068,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="59"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -2953,11 +3098,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="78" t="str">
+      <c r="C4" s="42" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="79"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2974,12 +3119,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="78" t="str">
+      <c r="D5" s="42" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="79"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="43"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2996,14 +3141,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="81" t="str">
+      <c r="C6" s="45" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -3016,14 +3161,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="81" t="str">
+      <c r="C7" s="45" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="83"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -3035,40 +3180,40 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="81" t="str">
+      <c r="C8" s="45" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="83"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="47"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="81" t="str">
+      <c r="I8" s="45" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="90"/>
-      <c r="K8" s="83"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="47"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="81" t="str">
+      <c r="D9" s="45" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="83"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -3080,34 +3225,34 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="91" t="str">
+      <c r="C10" s="61" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="83"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="47"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="52" t="str">
+      <c r="C11" s="48" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -3119,16 +3264,16 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="52" t="str">
+      <c r="C12" s="48" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="54"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -3140,65 +3285,65 @@
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="66" t="str">
+      <c r="C13" s="63" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="68"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="66" t="str">
+      <c r="K13" s="63" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="68"/>
+      <c r="L13" s="64"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="69" t="str">
+      <c r="C14" s="74" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="71"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="76"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="69" t="str">
+      <c r="I14" s="74" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="71"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="76"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="69" t="str">
+      <c r="C15" s="74" t="str">
         <f>'Drug Information'!$A24</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="71"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="76"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3208,20 +3353,20 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="72" t="s">
+      <c r="E16" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="74"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="79"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
@@ -3230,34 +3375,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="38" t="str">
+      <c r="E17" s="83" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="85"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="38" t="str">
+      <c r="C18" s="83" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A27</f>
@@ -3265,25 +3410,25 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="43" t="str">
+      <c r="C19" s="57" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="45"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="43" t="str">
+      <c r="I19" s="57" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="59"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3292,14 +3437,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="48" t="str">
+      <c r="E20" s="90" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="93"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -3309,12 +3454,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="60" t="str">
+      <c r="B21" s="67" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3333,11 +3478,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="46" t="str">
+      <c r="C22" s="88" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="89"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3358,13 +3503,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="55" t="str">
+      <c r="B23" s="94" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -3384,12 +3529,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="63" t="str">
+      <c r="B24" s="70" t="str">
         <f>'Drug Information'!$A35</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3404,15 +3549,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="34" t="str">
+      <c r="B25" s="80" t="str">
         <f>'Drug Information'!$A38</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -3445,24 +3590,43 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -3479,25 +3643,6 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add "Colour" column to spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/assets/antibiogram.xlsx
+++ b/docs/assets/antibiogram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bacteria Information" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="110">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -309,13 +309,70 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>(68, 114, 196)</t>
+  </si>
+  <si>
+    <t>(128, 96, 0)</t>
+  </si>
+  <si>
+    <t>(144, 86, 145)</t>
+  </si>
+  <si>
+    <t>(192, 0, 0)</t>
+  </si>
+  <si>
+    <t>(128, 128, 128)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>(224, 224, 224)</t>
+  </si>
+  <si>
+    <t>(204, 229, 255)</t>
+  </si>
+  <si>
+    <t>(169, 169, 169)</t>
+  </si>
+  <si>
+    <t>(255, 235, 204)</t>
+  </si>
+  <si>
+    <t>(255, 255, 153)</t>
+  </si>
+  <si>
+    <t>(224, 255, 224)</t>
+  </si>
+  <si>
+    <t>(255, 204, 153)</t>
+  </si>
+  <si>
+    <t>(153, 255, 255)</t>
+  </si>
+  <si>
+    <t>(255, 255, 204)</t>
+  </si>
+  <si>
+    <t>(255, 204, 204)</t>
+  </si>
+  <si>
+    <t>(204, 204, 255)</t>
+  </si>
+  <si>
+    <t>(153, 255, 153)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -400,6 +457,18 @@
       <color theme="0"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF8F8F2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE6DB74"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="21">
@@ -678,7 +747,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -785,6 +854,129 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -794,9 +986,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -815,15 +1004,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -842,15 +1022,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -860,107 +1031,11 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -968,10 +1043,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <font>
         <b val="0"/>
@@ -1006,7 +1078,8 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1061,6 +1134,30 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1213,62 +1310,64 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AO16" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A1:AO16"/>
-  <tableColumns count="41">
-    <tableColumn id="1" name="Group" dataDxfId="45"/>
-    <tableColumn id="2" name="Name" dataDxfId="44"/>
-    <tableColumn id="41" name="Include" dataDxfId="0"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="43"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="42"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="41"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="40"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="39"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="38"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="37"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="36"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="35"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="34"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="33"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="32"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="31"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="30"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="29"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="28"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="27"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="26"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="25"/>
-    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="24"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="23"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="22"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="21"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="20"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="19"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="18"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="17"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="16"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="15"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="14"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="13"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="12"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="11"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="10"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="9"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="8"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="7"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AP16" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:AP16"/>
+  <tableColumns count="42">
+    <tableColumn id="1" name="Group" dataDxfId="47"/>
+    <tableColumn id="2" name="Name" dataDxfId="46"/>
+    <tableColumn id="41" name="Include" dataDxfId="45"/>
+    <tableColumn id="42" name="Colour" dataDxfId="6"/>
+    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="44"/>
+    <tableColumn id="4" name="Naficillin" dataDxfId="43"/>
+    <tableColumn id="5" name="Oxacillin" dataDxfId="42"/>
+    <tableColumn id="6" name="Flucloxacillin" dataDxfId="41"/>
+    <tableColumn id="7" name="Ampicillin" dataDxfId="40"/>
+    <tableColumn id="8" name="Amoxicillin" dataDxfId="39"/>
+    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="38"/>
+    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="37"/>
+    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="36"/>
+    <tableColumn id="12" name="Cefazolin" dataDxfId="35"/>
+    <tableColumn id="13" name="Cefalexin" dataDxfId="34"/>
+    <tableColumn id="14" name="Cefuroxime" dataDxfId="33"/>
+    <tableColumn id="15" name="Cephotetan" dataDxfId="32"/>
+    <tableColumn id="16" name="Cefoxitin" dataDxfId="31"/>
+    <tableColumn id="17" name="Cefotaxime" dataDxfId="30"/>
+    <tableColumn id="18" name="Ceftriaxone" dataDxfId="29"/>
+    <tableColumn id="19" name="Ceftazidime" dataDxfId="28"/>
+    <tableColumn id="20" name="Cefepime" dataDxfId="27"/>
+    <tableColumn id="21" name="Ceftaroline" dataDxfId="26"/>
+    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="25"/>
+    <tableColumn id="22" name="Ertapenem" dataDxfId="24"/>
+    <tableColumn id="23" name="Imipenem" dataDxfId="23"/>
+    <tableColumn id="24" name="Meropenem" dataDxfId="22"/>
+    <tableColumn id="25" name="Aztreonam" dataDxfId="21"/>
+    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="20"/>
+    <tableColumn id="27" name="Levofloxacin" dataDxfId="19"/>
+    <tableColumn id="28" name="Moxifloxacin" dataDxfId="18"/>
+    <tableColumn id="29" name="Gentamicin" dataDxfId="17"/>
+    <tableColumn id="30" name="Tobramycin" dataDxfId="16"/>
+    <tableColumn id="31" name="Amikacin" dataDxfId="15"/>
+    <tableColumn id="32" name="Azithromycin" dataDxfId="14"/>
+    <tableColumn id="33" name="Clindamycin" dataDxfId="13"/>
+    <tableColumn id="34" name="Doxycycline" dataDxfId="12"/>
+    <tableColumn id="35" name="Vancomycin" dataDxfId="11"/>
+    <tableColumn id="36" name="Daptomycin" dataDxfId="10"/>
+    <tableColumn id="37" name="Linezolid" dataDxfId="9"/>
+    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="8"/>
+    <tableColumn id="39" name="Metronidazole" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:C39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:C39"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:D39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D39"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Drug Name" dataDxfId="3"/>
     <tableColumn id="2" name="Drug Class" dataDxfId="2"/>
-    <tableColumn id="3" name="Include" dataDxfId="1"/>
+    <tableColumn id="4" name="Colour" dataDxfId="1"/>
+    <tableColumn id="3" name="Include" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1529,7 +1628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1540,12 +1639,12 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AO16"/>
+  <dimension ref="A1:AP23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="10320" ySplit="7875" topLeftCell="A25"/>
-      <selection activeCell="D21" sqref="D21"/>
-      <selection pane="topRight" activeCell="U18" sqref="U18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="10320" ySplit="7875" topLeftCell="A25" activePane="topRight"/>
+      <selection activeCell="D2" sqref="D2"/>
+      <selection pane="topRight" activeCell="C21" sqref="C21"/>
       <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
       <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
@@ -1593,7 +1692,7 @@
     <col min="41" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>78</v>
       </c>
@@ -1604,121 +1703,124 @@
         <v>89</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="S1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="33" t="s">
+      <c r="AE1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AF1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AG1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="AI1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="AM1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AN1" s="33" t="s">
+      <c r="AO1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="AO1" s="33" t="s">
+      <c r="AP1" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -1728,10 +1830,10 @@
       <c r="C2" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="V2" s="33">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="33">
+      <c r="D2" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="33">
         <v>1</v>
       </c>
       <c r="AJ2" s="33">
@@ -1749,8 +1851,11 @@
       <c r="AN2" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AO2" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
@@ -1760,8 +1865,8 @@
       <c r="C3" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="33">
-        <v>1</v>
+      <c r="D3" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="F3" s="33">
         <v>1</v>
@@ -1769,7 +1874,7 @@
       <c r="G3" s="33">
         <v>1</v>
       </c>
-      <c r="J3" s="33">
+      <c r="H3" s="33">
         <v>1</v>
       </c>
       <c r="K3" s="33">
@@ -1799,13 +1904,13 @@
       <c r="S3" s="33">
         <v>1</v>
       </c>
-      <c r="U3" s="33">
+      <c r="T3" s="33">
         <v>1</v>
       </c>
       <c r="V3" s="33">
         <v>1</v>
       </c>
-      <c r="X3" s="33">
+      <c r="W3" s="33">
         <v>1</v>
       </c>
       <c r="Y3" s="33">
@@ -1814,7 +1919,7 @@
       <c r="Z3" s="33">
         <v>1</v>
       </c>
-      <c r="AB3" s="33">
+      <c r="AA3" s="33">
         <v>1</v>
       </c>
       <c r="AC3" s="33">
@@ -1823,7 +1928,7 @@
       <c r="AD3" s="33">
         <v>1</v>
       </c>
-      <c r="AH3" s="33">
+      <c r="AE3" s="33">
         <v>1</v>
       </c>
       <c r="AI3" s="33">
@@ -1844,8 +1949,11 @@
       <c r="AN3" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AO3" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
@@ -1855,8 +1963,8 @@
       <c r="C4" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="33">
-        <v>1</v>
+      <c r="D4" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="E4" s="33">
         <v>1</v>
@@ -1924,13 +2032,13 @@
       <c r="Z4" s="33">
         <v>1</v>
       </c>
-      <c r="AC4" s="33">
+      <c r="AA4" s="33">
         <v>1</v>
       </c>
       <c r="AD4" s="33">
         <v>1</v>
       </c>
-      <c r="AH4" s="33">
+      <c r="AE4" s="33">
         <v>1</v>
       </c>
       <c r="AI4" s="33">
@@ -1951,8 +2059,11 @@
       <c r="AN4" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AO4" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>80</v>
       </c>
@@ -1962,8 +2073,8 @@
       <c r="C5" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="33">
-        <v>1</v>
+      <c r="D5" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="I5" s="33">
         <v>1</v>
@@ -2040,14 +2151,17 @@
       <c r="AG5" s="33">
         <v>1</v>
       </c>
-      <c r="AJ5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AN5" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AH5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>80</v>
       </c>
@@ -2057,8 +2171,8 @@
       <c r="C6" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="33">
-        <v>1</v>
+      <c r="D6" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="I6" s="33">
         <v>1</v>
@@ -2135,11 +2249,14 @@
       <c r="AG6" s="33">
         <v>1</v>
       </c>
-      <c r="AN6" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AH6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>80</v>
       </c>
@@ -2149,8 +2266,8 @@
       <c r="C7" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="33">
-        <v>1</v>
+      <c r="D7" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="K7" s="33">
         <v>1</v>
@@ -2221,11 +2338,14 @@
       <c r="AG7" s="33">
         <v>1</v>
       </c>
-      <c r="AN7" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AH7" s="33">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>80</v>
       </c>
@@ -2235,19 +2355,19 @@
       <c r="C8" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="33">
-        <v>1</v>
-      </c>
-      <c r="T8" s="33">
+      <c r="D8" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="33">
         <v>1</v>
       </c>
       <c r="U8" s="33">
         <v>1</v>
       </c>
-      <c r="W8" s="33">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="33">
+      <c r="V8" s="33">
+        <v>1</v>
+      </c>
+      <c r="X8" s="33">
         <v>1</v>
       </c>
       <c r="Z8" s="33">
@@ -2262,7 +2382,7 @@
       <c r="AC8" s="33">
         <v>1</v>
       </c>
-      <c r="AE8" s="33">
+      <c r="AD8" s="33">
         <v>1</v>
       </c>
       <c r="AF8" s="33">
@@ -2271,8 +2391,11 @@
       <c r="AG8" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AH8" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>80</v>
       </c>
@@ -2280,24 +2403,24 @@
         <v>5</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="L9" s="33">
-        <v>1</v>
-      </c>
-      <c r="R9" s="33">
+        <v>97</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" s="33">
         <v>1</v>
       </c>
       <c r="S9" s="33">
         <v>1</v>
       </c>
-      <c r="U9" s="33">
+      <c r="T9" s="33">
         <v>1</v>
       </c>
       <c r="V9" s="33">
         <v>1</v>
       </c>
-      <c r="X9" s="33">
+      <c r="W9" s="33">
         <v>1</v>
       </c>
       <c r="Y9" s="33">
@@ -2327,7 +2450,7 @@
       <c r="AG9" s="33">
         <v>1</v>
       </c>
-      <c r="AL9" s="33">
+      <c r="AH9" s="33">
         <v>1</v>
       </c>
       <c r="AM9" s="33">
@@ -2336,8 +2459,11 @@
       <c r="AN9" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AO9" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>81</v>
       </c>
@@ -2347,13 +2473,13 @@
       <c r="C10" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="S10" s="33">
-        <v>1</v>
-      </c>
-      <c r="U10" s="33">
-        <v>1</v>
-      </c>
-      <c r="X10" s="33">
+      <c r="D10" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="T10" s="33">
+        <v>1</v>
+      </c>
+      <c r="V10" s="33">
         <v>1</v>
       </c>
       <c r="Y10" s="33">
@@ -2374,8 +2500,11 @@
       <c r="AD10" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AE10" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
@@ -2385,25 +2514,25 @@
       <c r="C11" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="33">
-        <v>1</v>
+      <c r="D11" s="33" t="s">
+        <v>94</v>
       </c>
       <c r="I11" s="33">
         <v>1</v>
       </c>
-      <c r="L11" s="33">
-        <v>1</v>
-      </c>
-      <c r="R11" s="33">
+      <c r="J11" s="33">
+        <v>1</v>
+      </c>
+      <c r="M11" s="33">
         <v>1</v>
       </c>
       <c r="S11" s="33">
         <v>1</v>
       </c>
-      <c r="U11" s="33">
-        <v>1</v>
-      </c>
-      <c r="X11" s="33">
+      <c r="T11" s="33">
+        <v>1</v>
+      </c>
+      <c r="V11" s="33">
         <v>1</v>
       </c>
       <c r="Y11" s="33">
@@ -2424,17 +2553,20 @@
       <c r="AD11" s="33">
         <v>1</v>
       </c>
-      <c r="AH11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AN11" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AE11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
@@ -2444,8 +2576,8 @@
       <c r="C12" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="33">
-        <v>1</v>
+      <c r="D12" s="33" t="s">
+        <v>93</v>
       </c>
       <c r="K12" s="33">
         <v>1</v>
@@ -2453,13 +2585,13 @@
       <c r="L12" s="33">
         <v>1</v>
       </c>
-      <c r="P12" s="33">
+      <c r="M12" s="33">
         <v>1</v>
       </c>
       <c r="Q12" s="33">
         <v>1</v>
       </c>
-      <c r="X12" s="33">
+      <c r="R12" s="33">
         <v>1</v>
       </c>
       <c r="Y12" s="33">
@@ -2468,17 +2600,20 @@
       <c r="Z12" s="33">
         <v>1</v>
       </c>
-      <c r="AD12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AA12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>15</v>
       </c>
@@ -2488,31 +2623,34 @@
       <c r="C13" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="AC13" s="33">
-        <v>1</v>
+      <c r="D13" s="33" t="s">
+        <v>96</v>
       </c>
       <c r="AD13" s="33">
         <v>1</v>
       </c>
-      <c r="AH13" s="33">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AE13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="W14" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="X14" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>85</v>
       </c>
@@ -2520,7 +2658,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>86</v>
       </c>
@@ -2528,10 +2666,26 @@
         <v>90</v>
       </c>
     </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="97"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="98"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="98"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="98"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="98"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2541,10 +2695,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2552,419 +2706,581 @@
     <col min="1" max="1" width="31.875" style="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.875" style="32" customWidth="1"/>
     <col min="3" max="3" width="17.875" style="32" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="32"/>
+    <col min="4" max="4" width="9" style="32"/>
+    <col min="5" max="5" width="16.875" style="32" customWidth="1"/>
+    <col min="6" max="6" width="41.625" style="32" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" s="97"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="98"/>
+      <c r="G2" s="97"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="37"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="37"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="37"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="37"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="98"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>66</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="37"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="37"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="37"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="98"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="37"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="37"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>52</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>73</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="37" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2986,7 +3302,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C49" sqref="C49"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3011,23 +3327,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="51" t="s">
+      <c r="C1" s="92"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="39" t="s">
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="65" t="s">
+      <c r="K1" s="81"/>
+      <c r="L1" s="62" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -3068,7 +3384,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="66"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -3098,11 +3414,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="42" t="str">
+      <c r="C4" s="82" t="str">
         <f>'Drug Information'!$A5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3119,12 +3435,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="42" t="str">
+      <c r="D5" s="82" t="str">
         <f>'Drug Information'!$A7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="43"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="83"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -3141,14 +3457,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="45" t="str">
+      <c r="C6" s="85" t="str">
         <f>'Drug Information'!$A11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="87"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -3161,14 +3477,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="45" t="str">
+      <c r="C7" s="85" t="str">
         <f>'Drug Information'!$A15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="47"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="87"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -3184,21 +3500,21 @@
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="45" t="str">
+      <c r="C8" s="85" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="47"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="87"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="45" t="str">
+      <c r="I8" s="85" t="str">
         <f>'Drug Information'!$A17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="60"/>
-      <c r="K8" s="47"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="87"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
@@ -3206,14 +3522,14 @@
       <c r="A9" s="41"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="45" t="str">
+      <c r="D9" s="85" t="str">
         <f>'Drug Information'!$A18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="47"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="87"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -3225,18 +3541,18 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="61" t="str">
+      <c r="C10" s="95" t="str">
         <f>'Drug Information'!$A19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="47"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="87"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
@@ -3245,14 +3561,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="48" t="str">
+      <c r="C11" s="56" t="str">
         <f>'Drug Information'!$A8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -3266,14 +3582,14 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="48" t="str">
+      <c r="C12" s="56" t="str">
         <f>'Drug Information'!$A9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="50"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -3287,22 +3603,22 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="63" t="str">
+      <c r="C13" s="70" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="64"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="72"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="63" t="str">
+      <c r="K13" s="70" t="str">
         <f>'Drug Information'!$A10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="64"/>
+      <c r="L13" s="72"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3310,40 +3626,40 @@
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="74" t="str">
+      <c r="C14" s="73" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="76"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="75"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="74" t="str">
+      <c r="I14" s="73" t="str">
         <f>'Drug Information'!$A22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="76"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="75"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="41"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="74" t="str">
+      <c r="C15" s="73" t="str">
         <f>'Drug Information'!$A24</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="76"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="75"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3353,15 +3669,15 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="79"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="78"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
@@ -3375,34 +3691,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="83" t="str">
+      <c r="E17" s="42" t="str">
         <f>'Drug Information'!$A26</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="85"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="44"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="83" t="str">
+      <c r="C18" s="42" t="str">
         <f>'Drug Information'!$A27</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="87"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$A27</f>
@@ -3412,23 +3728,23 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="57" t="str">
+      <c r="C19" s="47" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="59"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="57" t="str">
+      <c r="I19" s="47" t="str">
         <f>'Drug Information'!$A28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="59"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="49"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3437,14 +3753,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="90" t="str">
+      <c r="E20" s="52" t="str">
         <f>'Drug Information'!$A31</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="93"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="55"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -3454,12 +3770,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="67" t="str">
+      <c r="B21" s="64" t="str">
         <f>'Drug Information'!$A33</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="69"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="66"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3478,11 +3794,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="88" t="str">
+      <c r="C22" s="50" t="str">
         <f>'Drug Information'!$A32</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="89"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3503,13 +3819,13 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="94" t="str">
+      <c r="B23" s="59" t="str">
         <f>'Drug Information'!$A34</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="96"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -3529,12 +3845,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="70" t="str">
+      <c r="B24" s="67" t="str">
         <f>'Drug Information'!$A35</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="72"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="69"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3549,15 +3865,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="80" t="str">
+      <c r="B25" s="38" t="str">
         <f>'Drug Information'!$A38</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="82"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="40"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -3590,43 +3906,24 @@
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -3643,6 +3940,25 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix colour mapping from Excel file, add clearer terminal messages
</commit_message>
<xml_diff>
--- a/docs/assets/antibiogram.xlsx
+++ b/docs/assets/antibiogram.xlsx
@@ -854,31 +854,67 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -890,40 +926,19 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,15 +965,9 @@
     <xf numFmtId="0" fontId="10" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -977,65 +986,56 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1044,6 +1044,24 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1080,24 +1098,6 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1316,45 +1316,45 @@
     <tableColumn id="1" name="Group" dataDxfId="47"/>
     <tableColumn id="2" name="Name" dataDxfId="46"/>
     <tableColumn id="41" name="Include" dataDxfId="45"/>
-    <tableColumn id="42" name="Colour" dataDxfId="6"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="44"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="43"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="42"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="41"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="40"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="39"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="38"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="37"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="36"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="35"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="34"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="33"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="32"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="31"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="30"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="29"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="28"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="27"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="26"/>
-    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="25"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="24"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="23"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="22"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="21"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="20"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="19"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="18"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="17"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="16"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="15"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="14"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="13"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="12"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="11"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="10"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="9"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="8"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="7"/>
+    <tableColumn id="42" name="Colour" dataDxfId="44"/>
+    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="43"/>
+    <tableColumn id="4" name="Naficillin" dataDxfId="42"/>
+    <tableColumn id="5" name="Oxacillin" dataDxfId="41"/>
+    <tableColumn id="6" name="Flucloxacillin" dataDxfId="40"/>
+    <tableColumn id="7" name="Ampicillin" dataDxfId="39"/>
+    <tableColumn id="8" name="Amoxicillin" dataDxfId="38"/>
+    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="37"/>
+    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="36"/>
+    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="35"/>
+    <tableColumn id="12" name="Cefazolin" dataDxfId="34"/>
+    <tableColumn id="13" name="Cefalexin" dataDxfId="33"/>
+    <tableColumn id="14" name="Cefuroxime" dataDxfId="32"/>
+    <tableColumn id="15" name="Cephotetan" dataDxfId="31"/>
+    <tableColumn id="16" name="Cefoxitin" dataDxfId="30"/>
+    <tableColumn id="17" name="Cefotaxime" dataDxfId="29"/>
+    <tableColumn id="18" name="Ceftriaxone" dataDxfId="28"/>
+    <tableColumn id="19" name="Ceftazidime" dataDxfId="27"/>
+    <tableColumn id="20" name="Cefepime" dataDxfId="26"/>
+    <tableColumn id="21" name="Ceftaroline" dataDxfId="25"/>
+    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="24"/>
+    <tableColumn id="22" name="Ertapenem" dataDxfId="23"/>
+    <tableColumn id="23" name="Imipenem" dataDxfId="22"/>
+    <tableColumn id="24" name="Meropenem" dataDxfId="21"/>
+    <tableColumn id="25" name="Aztreonam" dataDxfId="20"/>
+    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="19"/>
+    <tableColumn id="27" name="Levofloxacin" dataDxfId="18"/>
+    <tableColumn id="28" name="Moxifloxacin" dataDxfId="17"/>
+    <tableColumn id="29" name="Gentamicin" dataDxfId="16"/>
+    <tableColumn id="30" name="Tobramycin" dataDxfId="15"/>
+    <tableColumn id="31" name="Amikacin" dataDxfId="14"/>
+    <tableColumn id="32" name="Azithromycin" dataDxfId="13"/>
+    <tableColumn id="33" name="Clindamycin" dataDxfId="12"/>
+    <tableColumn id="34" name="Doxycycline" dataDxfId="11"/>
+    <tableColumn id="35" name="Vancomycin" dataDxfId="10"/>
+    <tableColumn id="36" name="Daptomycin" dataDxfId="9"/>
+    <tableColumn id="37" name="Linezolid" dataDxfId="8"/>
+    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="7"/>
+    <tableColumn id="39" name="Metronidazole" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1364,10 +1364,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:D39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D39"/>
   <tableColumns count="4">
+    <tableColumn id="5" name="Drug Class" dataDxfId="0"/>
     <tableColumn id="1" name="Drug Name" dataDxfId="3"/>
-    <tableColumn id="2" name="Drug Class" dataDxfId="2"/>
-    <tableColumn id="4" name="Colour" dataDxfId="1"/>
-    <tableColumn id="3" name="Include" dataDxfId="0"/>
+    <tableColumn id="4" name="Colour" dataDxfId="2"/>
+    <tableColumn id="3" name="Include" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1628,7 +1628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2667,19 +2667,19 @@
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="97"/>
+      <c r="C19" s="38"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="98"/>
+      <c r="C20" s="39"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="98"/>
+      <c r="C21" s="39"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="98"/>
+      <c r="C22" s="39"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="98"/>
+      <c r="C23" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2698,7 +2698,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2714,10 +2714,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>53</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>91</v>
@@ -2725,14 +2725,14 @@
       <c r="D1" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="97"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>98</v>
@@ -2740,43 +2740,43 @@
       <c r="D2" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="98"/>
-      <c r="G2" s="97"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>28</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D3" s="37"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D4" s="37"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>28</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>98</v>
@@ -2784,29 +2784,29 @@
       <c r="D5" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>60</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>29</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D6" s="37"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>29</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>98</v>
@@ -2814,15 +2814,15 @@
       <c r="D7" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>34</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>99</v>
@@ -2830,29 +2830,29 @@
       <c r="D8" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="35" t="s">
         <v>50</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>34</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>99</v>
       </c>
       <c r="D9" s="37"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>99</v>
@@ -2860,15 +2860,15 @@
       <c r="D10" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>69</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>100</v>
@@ -2876,15 +2876,15 @@
       <c r="D11" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>100</v>
@@ -2892,15 +2892,15 @@
       <c r="D12" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>31</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>100</v>
@@ -2908,43 +2908,43 @@
       <c r="D13" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>31</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>100</v>
       </c>
       <c r="D14" s="37"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>100</v>
       </c>
       <c r="D15" s="37"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="31" t="s">
         <v>71</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>32</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>100</v>
@@ -2952,15 +2952,15 @@
       <c r="D16" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>7</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>32</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>100</v>
@@ -2968,15 +2968,15 @@
       <c r="D17" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>10</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>33</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>100</v>
@@ -2984,29 +2984,29 @@
       <c r="D18" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>9</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>33</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>100</v>
       </c>
       <c r="D19" s="37"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>72</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>74</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>100</v>
@@ -3014,15 +3014,15 @@
       <c r="D20" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="37" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>88</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>100</v>
@@ -3030,15 +3030,15 @@
       <c r="D21" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="98"/>
-      <c r="G21" s="98"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="31" t="s">
         <v>11</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>42</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>101</v>
@@ -3046,14 +3046,14 @@
       <c r="D22" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="G22" s="98"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="35" t="s">
         <v>62</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>42</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>101</v>
@@ -3062,10 +3062,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="31" t="s">
         <v>63</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>42</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>101</v>
@@ -3075,11 +3075,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="36" t="s">
         <v>43</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>12</v>
       </c>
       <c r="C25" s="32" t="s">
         <v>102</v>
@@ -3090,10 +3090,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>26</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>38</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>103</v>
@@ -3104,10 +3104,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="31" t="s">
         <v>13</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>38</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>103</v>
@@ -3117,11 +3117,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="36" t="s">
         <v>14</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>38</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>103</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>35</v>
       </c>
       <c r="C29" s="32" t="s">
         <v>104</v>
@@ -3146,10 +3146,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>64</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>35</v>
       </c>
       <c r="C30" s="32" t="s">
         <v>104</v>
@@ -3160,10 +3160,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="31" t="s">
         <v>65</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>35</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>104</v>
@@ -3174,10 +3174,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="31" t="s">
         <v>39</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>17</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>105</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="31" t="s">
         <v>52</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>19</v>
       </c>
       <c r="C33" s="32" t="s">
         <v>106</v>
@@ -3202,10 +3202,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="31" t="s">
         <v>45</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>16</v>
       </c>
       <c r="C34" s="32" t="s">
         <v>107</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="31" t="s">
         <v>27</v>
-      </c>
-      <c r="B35" s="31" t="s">
-        <v>36</v>
       </c>
       <c r="C35" s="32" t="s">
         <v>108</v>
@@ -3230,10 +3230,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="31" t="s">
         <v>73</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>75</v>
       </c>
       <c r="C36" s="32" t="s">
         <v>108</v>
@@ -3244,10 +3244,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="31" t="s">
         <v>76</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>77</v>
       </c>
       <c r="C37" s="32" t="s">
         <v>108</v>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="31" t="s">
         <v>55</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>37</v>
       </c>
       <c r="C38" s="32" t="s">
         <v>109</v>
@@ -3272,10 +3272,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="31" t="s">
         <v>25</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>24</v>
       </c>
       <c r="C39" s="32" t="s">
         <v>102</v>
@@ -3327,23 +3327,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="88" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="80" t="s">
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="81"/>
-      <c r="L1" s="62" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="67" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -3384,7 +3384,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="63"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -3396,7 +3396,7 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="str">
-        <f>'Drug Information'!$A2</f>
+        <f>'Drug Information'!$B2</f>
         <v>Benzylpenicillin</v>
       </c>
       <c r="E3" s="6"/>
@@ -3414,11 +3414,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="82" t="str">
-        <f>'Drug Information'!$A5</f>
+      <c r="C4" s="44" t="str">
+        <f>'Drug Information'!$B5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="45"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3435,18 +3435,18 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="82" t="str">
-        <f>'Drug Information'!$A7</f>
+      <c r="D5" s="44" t="str">
+        <f>'Drug Information'!$B7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="83"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="8" t="str">
-        <f>'Drug Information'!$A7</f>
+        <f>'Drug Information'!$B7</f>
         <v>Amoxicillin</v>
       </c>
       <c r="L5" s="6"/>
@@ -3457,14 +3457,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="85" t="str">
-        <f>'Drug Information'!$A11</f>
+      <c r="C6" s="47" t="str">
+        <f>'Drug Information'!$B11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="87"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -3477,59 +3477,59 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="85" t="str">
-        <f>'Drug Information'!$A15</f>
+      <c r="C7" s="47" t="str">
+        <f>'Drug Information'!$B15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="87"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="10" t="str">
-        <f>'Drug Information'!$A15</f>
+        <f>'Drug Information'!$B15</f>
         <v>Cefoxitin</v>
       </c>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="43" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="85" t="str">
-        <f>'Drug Information'!$A17</f>
+      <c r="C8" s="47" t="str">
+        <f>'Drug Information'!$B17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="87"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="85" t="str">
-        <f>'Drug Information'!$A17</f>
+      <c r="I8" s="47" t="str">
+        <f>'Drug Information'!$B17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="94"/>
-      <c r="K8" s="87"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="49"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="85" t="str">
-        <f>'Drug Information'!$A18</f>
+      <c r="D9" s="47" t="str">
+        <f>'Drug Information'!$B18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="87"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="49"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -3541,125 +3541,125 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="95" t="str">
-        <f>'Drug Information'!$A19</f>
+      <c r="C10" s="63" t="str">
+        <f>'Drug Information'!$B19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="87"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="56" t="str">
-        <f>'Drug Information'!$A8</f>
+      <c r="C11" s="50" t="str">
+        <f>'Drug Information'!$B8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="11" t="str">
-        <f>'Drug Information'!$A8</f>
+        <f>'Drug Information'!$B8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="56" t="str">
-        <f>'Drug Information'!$A9</f>
+      <c r="C12" s="50" t="str">
+        <f>'Drug Information'!$B9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="11" t="str">
-        <f>'Drug Information'!$A9</f>
+        <f>'Drug Information'!$B9</f>
         <v>Ampicillin/Sulbactam</v>
       </c>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="70" t="str">
-        <f>'Drug Information'!$A10</f>
+      <c r="C13" s="65" t="str">
+        <f>'Drug Information'!$B10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="72"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="66"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="70" t="str">
-        <f>'Drug Information'!$A10</f>
+      <c r="K13" s="65" t="str">
+        <f>'Drug Information'!$B10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="72"/>
+      <c r="L13" s="66"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="73" t="str">
-        <f>'Drug Information'!$A22</f>
+      <c r="C14" s="76" t="str">
+        <f>'Drug Information'!$B22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="75"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="78"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="73" t="str">
-        <f>'Drug Information'!$A22</f>
+      <c r="I14" s="76" t="str">
+        <f>'Drug Information'!$B22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="75"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="78"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="73" t="str">
-        <f>'Drug Information'!$A24</f>
+      <c r="C15" s="76" t="str">
+        <f>'Drug Information'!$B24</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="75"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="78"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3669,82 +3669,82 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="76" t="s">
+      <c r="E16" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="78"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="81"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="43" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="12" t="str">
-        <f>'Drug Information'!$A26</f>
+        <f>'Drug Information'!$B26</f>
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="42" t="str">
-        <f>'Drug Information'!$A26</f>
+      <c r="E17" s="85" t="str">
+        <f>'Drug Information'!$B26</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="44"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="87"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="42" t="str">
-        <f>'Drug Information'!$A27</f>
+      <c r="C18" s="85" t="str">
+        <f>'Drug Information'!$B27</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="89"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
-        <f>'Drug Information'!$A27</f>
+        <f>'Drug Information'!$B27</f>
         <v>Levofloxacin</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="47" t="str">
-        <f>'Drug Information'!$A28</f>
+      <c r="C19" s="59" t="str">
+        <f>'Drug Information'!$B28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="61"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="47" t="str">
-        <f>'Drug Information'!$A28</f>
+      <c r="I19" s="59" t="str">
+        <f>'Drug Information'!$B28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="49"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="61"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3753,14 +3753,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="52" t="str">
-        <f>'Drug Information'!$A31</f>
+      <c r="E20" s="92" t="str">
+        <f>'Drug Information'!$B31</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="55"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="95"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -3770,12 +3770,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="64" t="str">
-        <f>'Drug Information'!$A33</f>
+      <c r="B21" s="69" t="str">
+        <f>'Drug Information'!$B33</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3784,7 +3784,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="13" t="str">
-        <f>'Drug Information'!$A33</f>
+        <f>'Drug Information'!$B33</f>
         <v>Clindamycin</v>
       </c>
       <c r="M21" s="14"/>
@@ -3794,11 +3794,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="50" t="str">
-        <f>'Drug Information'!$A32</f>
+      <c r="C22" s="90" t="str">
+        <f>'Drug Information'!$B32</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="51"/>
+      <c r="D22" s="91"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3806,12 +3806,12 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="15" t="str">
-        <f>'Drug Information'!$A32</f>
+        <f>'Drug Information'!$B32</f>
         <v>Azithromycin</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="16" t="str">
-        <f>'Drug Information'!$A32</f>
+        <f>'Drug Information'!$B32</f>
         <v>Azithromycin</v>
       </c>
     </row>
@@ -3819,25 +3819,25 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="59" t="str">
-        <f>'Drug Information'!$A34</f>
+      <c r="B23" s="96" t="str">
+        <f>'Drug Information'!$B34</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="61"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="98"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="17" t="str">
-        <f>'Drug Information'!$A34</f>
+        <f>'Drug Information'!$B34</f>
         <v>Doxycycline</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="17" t="str">
-        <f>'Drug Information'!$A34</f>
+        <f>'Drug Information'!$B34</f>
         <v>Doxycycline</v>
       </c>
     </row>
@@ -3845,12 +3845,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="67" t="str">
-        <f>'Drug Information'!$A35</f>
+      <c r="B24" s="72" t="str">
+        <f>'Drug Information'!$B35</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="74"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3865,15 +3865,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="38" t="str">
-        <f>'Drug Information'!$A38</f>
+      <c r="B25" s="82" t="str">
+        <f>'Drug Information'!$B38</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="84"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -3900,30 +3900,49 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="20" t="str">
-        <f>'Drug Information'!$A39</f>
+        <f>'Drug Information'!$B39</f>
         <v>Metronidazole</v>
       </c>
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="E16:K16"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A11:A13"/>
@@ -3940,25 +3959,6 @@
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="E16:K16"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E17:K17"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add further drug information and tweak colours
</commit_message>
<xml_diff>
--- a/docs/assets/antibiogram.xlsx
+++ b/docs/assets/antibiogram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="Bacteria Information" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="116">
   <si>
     <t>Gram positive cocci</t>
   </si>
@@ -296,9 +296,6 @@
     <t>CPE</t>
   </si>
   <si>
-    <t>VRE</t>
-  </si>
-  <si>
     <t>Ceftazidime/Avibactam</t>
   </si>
   <si>
@@ -329,18 +326,12 @@
     <t>(128, 128, 128)</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>(224, 224, 224)</t>
   </si>
   <si>
     <t>(204, 229, 255)</t>
   </si>
   <si>
-    <t>(169, 169, 169)</t>
-  </si>
-  <si>
     <t>(255, 235, 204)</t>
   </si>
   <si>
@@ -366,6 +357,33 @@
   </si>
   <si>
     <t>(153, 255, 153)</t>
+  </si>
+  <si>
+    <t>Ceftazidime-Avibactam</t>
+  </si>
+  <si>
+    <t>Ampicillin-Sulbactam</t>
+  </si>
+  <si>
+    <t>Enterococcus</t>
+  </si>
+  <si>
+    <t>Clarithromycin</t>
+  </si>
+  <si>
+    <t>Nitrofurantoin</t>
+  </si>
+  <si>
+    <t>Nitrofurans</t>
+  </si>
+  <si>
+    <t>(200, 200, 200)</t>
+  </si>
+  <si>
+    <t>(58, 196, 58)</t>
+  </si>
+  <si>
+    <t>(219, 169, 82)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +606,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -842,24 +860,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1036,6 +1051,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1043,7 +1067,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="52">
     <dxf>
       <font>
         <b val="0"/>
@@ -1060,24 +1084,12 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1098,6 +1110,30 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1310,64 +1346,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AP16" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:AP16"/>
-  <tableColumns count="42">
-    <tableColumn id="1" name="Group" dataDxfId="47"/>
-    <tableColumn id="2" name="Name" dataDxfId="46"/>
-    <tableColumn id="41" name="Include" dataDxfId="45"/>
-    <tableColumn id="42" name="Colour" dataDxfId="44"/>
-    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="43"/>
-    <tableColumn id="4" name="Naficillin" dataDxfId="42"/>
-    <tableColumn id="5" name="Oxacillin" dataDxfId="41"/>
-    <tableColumn id="6" name="Flucloxacillin" dataDxfId="40"/>
-    <tableColumn id="7" name="Ampicillin" dataDxfId="39"/>
-    <tableColumn id="8" name="Amoxicillin" dataDxfId="38"/>
-    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="37"/>
-    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="36"/>
-    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="35"/>
-    <tableColumn id="12" name="Cefazolin" dataDxfId="34"/>
-    <tableColumn id="13" name="Cefalexin" dataDxfId="33"/>
-    <tableColumn id="14" name="Cefuroxime" dataDxfId="32"/>
-    <tableColumn id="15" name="Cephotetan" dataDxfId="31"/>
-    <tableColumn id="16" name="Cefoxitin" dataDxfId="30"/>
-    <tableColumn id="17" name="Cefotaxime" dataDxfId="29"/>
-    <tableColumn id="18" name="Ceftriaxone" dataDxfId="28"/>
-    <tableColumn id="19" name="Ceftazidime" dataDxfId="27"/>
-    <tableColumn id="20" name="Cefepime" dataDxfId="26"/>
-    <tableColumn id="21" name="Ceftaroline" dataDxfId="25"/>
-    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="24"/>
-    <tableColumn id="22" name="Ertapenem" dataDxfId="23"/>
-    <tableColumn id="23" name="Imipenem" dataDxfId="22"/>
-    <tableColumn id="24" name="Meropenem" dataDxfId="21"/>
-    <tableColumn id="25" name="Aztreonam" dataDxfId="20"/>
-    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="19"/>
-    <tableColumn id="27" name="Levofloxacin" dataDxfId="18"/>
-    <tableColumn id="28" name="Moxifloxacin" dataDxfId="17"/>
-    <tableColumn id="29" name="Gentamicin" dataDxfId="16"/>
-    <tableColumn id="30" name="Tobramycin" dataDxfId="15"/>
-    <tableColumn id="31" name="Amikacin" dataDxfId="14"/>
-    <tableColumn id="32" name="Azithromycin" dataDxfId="13"/>
-    <tableColumn id="33" name="Clindamycin" dataDxfId="12"/>
-    <tableColumn id="34" name="Doxycycline" dataDxfId="11"/>
-    <tableColumn id="35" name="Vancomycin" dataDxfId="10"/>
-    <tableColumn id="36" name="Daptomycin" dataDxfId="9"/>
-    <tableColumn id="37" name="Linezolid" dataDxfId="8"/>
-    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="7"/>
-    <tableColumn id="39" name="Metronidazole" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:AR15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <autoFilter ref="A1:AR15"/>
+  <tableColumns count="44">
+    <tableColumn id="1" name="Group" dataDxfId="49"/>
+    <tableColumn id="2" name="Name" dataDxfId="48"/>
+    <tableColumn id="41" name="Include" dataDxfId="47"/>
+    <tableColumn id="42" name="Colour" dataDxfId="46"/>
+    <tableColumn id="3" name="Benzylpenicillin" dataDxfId="45"/>
+    <tableColumn id="4" name="Naficillin" dataDxfId="44"/>
+    <tableColumn id="5" name="Oxacillin" dataDxfId="43"/>
+    <tableColumn id="6" name="Flucloxacillin" dataDxfId="42"/>
+    <tableColumn id="7" name="Ampicillin" dataDxfId="41"/>
+    <tableColumn id="8" name="Amoxicillin" dataDxfId="40"/>
+    <tableColumn id="9" name="Amoxicillin-Clavulanic Acid" dataDxfId="39"/>
+    <tableColumn id="10" name="Ampicillin/Sulbactam" dataDxfId="38"/>
+    <tableColumn id="11" name="Piperacillin-Tazobactam" dataDxfId="37"/>
+    <tableColumn id="12" name="Cefazolin" dataDxfId="36"/>
+    <tableColumn id="13" name="Cefalexin" dataDxfId="35"/>
+    <tableColumn id="14" name="Cefuroxime" dataDxfId="34"/>
+    <tableColumn id="15" name="Cephotetan" dataDxfId="33"/>
+    <tableColumn id="16" name="Cefoxitin" dataDxfId="32"/>
+    <tableColumn id="17" name="Cefotaxime" dataDxfId="31"/>
+    <tableColumn id="18" name="Ceftriaxone" dataDxfId="30"/>
+    <tableColumn id="19" name="Ceftazidime" dataDxfId="29"/>
+    <tableColumn id="20" name="Cefepime" dataDxfId="28"/>
+    <tableColumn id="21" name="Ceftaroline" dataDxfId="27"/>
+    <tableColumn id="40" name="Ceftazidime/Avibactam" dataDxfId="26"/>
+    <tableColumn id="22" name="Ertapenem" dataDxfId="25"/>
+    <tableColumn id="23" name="Imipenem" dataDxfId="24"/>
+    <tableColumn id="24" name="Meropenem" dataDxfId="23"/>
+    <tableColumn id="25" name="Aztreonam" dataDxfId="22"/>
+    <tableColumn id="26" name="Ciprofloxacin" dataDxfId="21"/>
+    <tableColumn id="27" name="Levofloxacin" dataDxfId="20"/>
+    <tableColumn id="28" name="Moxifloxacin" dataDxfId="19"/>
+    <tableColumn id="29" name="Gentamicin" dataDxfId="18"/>
+    <tableColumn id="30" name="Tobramycin" dataDxfId="17"/>
+    <tableColumn id="31" name="Amikacin" dataDxfId="16"/>
+    <tableColumn id="32" name="Azithromycin" dataDxfId="15"/>
+    <tableColumn id="43" name="Clarithromycin" dataDxfId="4"/>
+    <tableColumn id="33" name="Clindamycin" dataDxfId="14"/>
+    <tableColumn id="34" name="Doxycycline" dataDxfId="13"/>
+    <tableColumn id="35" name="Vancomycin" dataDxfId="12"/>
+    <tableColumn id="36" name="Daptomycin" dataDxfId="11"/>
+    <tableColumn id="37" name="Linezolid" dataDxfId="10"/>
+    <tableColumn id="38" name="Trimethoprim/Sulfamethoxazole" dataDxfId="9"/>
+    <tableColumn id="39" name="Metronidazole" dataDxfId="8"/>
+    <tableColumn id="44" name="Nitrofurantoin" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:D39" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="drug_info" displayName="drug_info" ref="A1:D41" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:D41"/>
   <tableColumns count="4">
-    <tableColumn id="5" name="Drug Class" dataDxfId="0"/>
-    <tableColumn id="1" name="Drug Name" dataDxfId="3"/>
-    <tableColumn id="4" name="Colour" dataDxfId="2"/>
-    <tableColumn id="3" name="Include" dataDxfId="1"/>
+    <tableColumn id="5" name="Drug Class" dataDxfId="2"/>
+    <tableColumn id="1" name="Drug Name" dataDxfId="0"/>
+    <tableColumn id="4" name="Colour" dataDxfId="1"/>
+    <tableColumn id="3" name="Include" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1639,14 +1677,12 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AP23"/>
+  <dimension ref="A1:AR21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="10320" ySplit="7875" topLeftCell="A25" activePane="topRight"/>
-      <selection activeCell="D2" sqref="D2"/>
-      <selection pane="topRight" activeCell="C21" sqref="C21"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="9090" topLeftCell="AA1"/>
+      <selection activeCell="D12" sqref="D12"/>
+      <selection pane="topRight" activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1687,12 +1723,12 @@
     <col min="35" max="35" width="13" style="33" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="13.25" style="33" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="31.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13" style="33" customWidth="1"/>
     <col min="40" max="40" width="15.5" style="33" bestFit="1" customWidth="1"/>
     <col min="41" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>78</v>
       </c>
@@ -1700,10 +1736,10 @@
         <v>79</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>48</v>
@@ -1763,7 +1799,7 @@
         <v>72</v>
       </c>
       <c r="X1" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y1" s="33" t="s">
         <v>11</v>
@@ -1799,28 +1835,34 @@
         <v>39</v>
       </c>
       <c r="AJ1" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AM1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="AN1" s="33" t="s">
+      <c r="AO1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="AO1" s="33" t="s">
+      <c r="AP1" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="AP1" s="33" t="s">
+      <c r="AQ1" s="33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AR1" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -1828,17 +1870,14 @@
         <v>1</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="W2" s="33">
         <v>1</v>
       </c>
-      <c r="AJ2" s="33">
-        <v>1</v>
-      </c>
       <c r="AK2" s="33">
         <v>1</v>
       </c>
@@ -1854,8 +1893,11 @@
       <c r="AO2" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP2" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
@@ -1863,10 +1905,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="33">
         <v>1</v>
@@ -1934,9 +1976,6 @@
       <c r="AI3" s="33">
         <v>1</v>
       </c>
-      <c r="AJ3" s="33">
-        <v>1</v>
-      </c>
       <c r="AK3" s="33">
         <v>1</v>
       </c>
@@ -1952,8 +1991,11 @@
       <c r="AO3" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP3" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
@@ -1961,10 +2003,10 @@
         <v>41</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="33">
         <v>1</v>
@@ -2062,16 +2104,19 @@
       <c r="AO4" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>80</v>
+      <c r="AP4" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A5" s="98" t="s">
+        <v>0</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>95</v>
@@ -2085,94 +2130,40 @@
       <c r="K5" s="33">
         <v>1</v>
       </c>
-      <c r="L5" s="33">
-        <v>1</v>
-      </c>
       <c r="M5" s="33">
         <v>1</v>
       </c>
-      <c r="N5" s="33">
-        <v>1</v>
-      </c>
-      <c r="O5" s="33">
-        <v>1</v>
-      </c>
-      <c r="P5" s="33">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="33">
-        <v>1</v>
-      </c>
-      <c r="R5" s="33">
-        <v>1</v>
-      </c>
-      <c r="S5" s="33">
-        <v>1</v>
-      </c>
-      <c r="T5" s="33">
-        <v>1</v>
-      </c>
-      <c r="U5" s="33">
-        <v>1</v>
-      </c>
-      <c r="V5" s="33">
-        <v>1</v>
-      </c>
       <c r="W5" s="33">
         <v>1</v>
       </c>
-      <c r="X5" s="33">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="33">
-        <v>1</v>
-      </c>
       <c r="AE5" s="33">
         <v>1</v>
       </c>
-      <c r="AF5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="33">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="33">
+      <c r="AM5" s="33">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="33">
         <v>1</v>
       </c>
       <c r="AO5" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AR5" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="33">
         <v>1</v>
@@ -2252,22 +2243,34 @@
       <c r="AH6" s="33">
         <v>1</v>
       </c>
-      <c r="AO6" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AL6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="I7" s="33">
+        <v>1</v>
+      </c>
+      <c r="J7" s="33">
+        <v>1</v>
       </c>
       <c r="K7" s="33">
         <v>1</v>
@@ -2341,35 +2344,68 @@
       <c r="AH7" s="33">
         <v>1</v>
       </c>
-      <c r="AO7" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP7" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="K8" s="33">
+        <v>1</v>
+      </c>
+      <c r="L8" s="33">
+        <v>1</v>
       </c>
       <c r="M8" s="33">
         <v>1</v>
       </c>
+      <c r="N8" s="33">
+        <v>1</v>
+      </c>
+      <c r="O8" s="33">
+        <v>1</v>
+      </c>
+      <c r="P8" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="33">
+        <v>1</v>
+      </c>
+      <c r="R8" s="33">
+        <v>1</v>
+      </c>
+      <c r="S8" s="33">
+        <v>1</v>
+      </c>
+      <c r="T8" s="33">
+        <v>1</v>
+      </c>
       <c r="U8" s="33">
         <v>1</v>
       </c>
       <c r="V8" s="33">
         <v>1</v>
       </c>
+      <c r="W8" s="33">
+        <v>1</v>
+      </c>
       <c r="X8" s="33">
         <v>1</v>
       </c>
+      <c r="Y8" s="33">
+        <v>1</v>
+      </c>
       <c r="Z8" s="33">
         <v>1</v>
       </c>
@@ -2385,6 +2421,9 @@
       <c r="AD8" s="33">
         <v>1</v>
       </c>
+      <c r="AE8" s="33">
+        <v>1</v>
+      </c>
       <c r="AF8" s="33">
         <v>1</v>
       </c>
@@ -2394,36 +2433,36 @@
       <c r="AH8" s="33">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP8" s="33">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>5</v>
+      <c r="B9" s="33" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M9" s="33">
         <v>1</v>
       </c>
-      <c r="S9" s="33">
-        <v>1</v>
-      </c>
-      <c r="T9" s="33">
+      <c r="U9" s="33">
         <v>1</v>
       </c>
       <c r="V9" s="33">
         <v>1</v>
       </c>
-      <c r="W9" s="33">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="33">
+      <c r="X9" s="33">
         <v>1</v>
       </c>
       <c r="Z9" s="33">
@@ -2441,9 +2480,6 @@
       <c r="AD9" s="33">
         <v>1</v>
       </c>
-      <c r="AE9" s="33">
-        <v>1</v>
-      </c>
       <c r="AF9" s="33">
         <v>1</v>
       </c>
@@ -2453,17 +2489,8 @@
       <c r="AH9" s="33">
         <v>1</v>
       </c>
-      <c r="AM9" s="33">
-        <v>1</v>
-      </c>
-      <c r="AN9" s="33">
-        <v>1</v>
-      </c>
-      <c r="AO9" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>81</v>
       </c>
@@ -2471,10 +2498,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T10" s="33">
         <v>1</v>
@@ -2504,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
@@ -2512,10 +2539,10 @@
         <v>44</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I11" s="33">
         <v>1</v>
@@ -2559,14 +2586,14 @@
       <c r="AI11" s="33">
         <v>1</v>
       </c>
-      <c r="AK11" s="33">
-        <v>1</v>
-      </c>
-      <c r="AO11" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AL11" s="33">
+        <v>1</v>
+      </c>
+      <c r="AP11" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
@@ -2574,10 +2601,10 @@
         <v>82</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K12" s="33">
         <v>1</v>
@@ -2606,14 +2633,14 @@
       <c r="AE12" s="33">
         <v>1</v>
       </c>
-      <c r="AJ12" s="33">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AK12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>15</v>
       </c>
@@ -2621,10 +2648,13 @@
         <v>83</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="AC13" s="33">
+        <v>1</v>
       </c>
       <c r="AD13" s="33">
         <v>1</v>
@@ -2635,51 +2665,46 @@
       <c r="AI13" s="33">
         <v>1</v>
       </c>
-      <c r="AK13" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="AJ13" s="33">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X14" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>90</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="36"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="38"/>
+      <c r="C19" s="37"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="39"/>
+      <c r="C20" s="37"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="39"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="39"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="39"/>
+      <c r="C21" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2695,18 +2720,18 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.875" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.875" style="32" customWidth="1"/>
+    <col min="2" max="2" width="41.875" style="100" customWidth="1"/>
     <col min="3" max="3" width="17.875" style="32" customWidth="1"/>
-    <col min="4" max="4" width="9" style="32"/>
+    <col min="4" max="4" width="13.75" style="32" customWidth="1"/>
     <col min="5" max="5" width="16.875" style="32" customWidth="1"/>
     <col min="6" max="6" width="41.625" style="32" customWidth="1"/>
     <col min="7" max="16384" width="9" style="32"/>
@@ -2716,572 +2741,598 @@
       <c r="A1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>54</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="38"/>
+        <v>90</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="34" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="38"/>
+        <v>96</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="37"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+        <v>96</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+        <v>96</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="34" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+        <v>96</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="37"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
+        <v>96</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="34" t="s">
         <v>61</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
+        <v>96</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="34" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
+        <v>97</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>50</v>
+      <c r="B9" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+        <v>97</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="34" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
+        <v>97</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="34" t="s">
         <v>69</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="34" t="s">
         <v>68</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="34" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="37"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D15" s="35"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="34" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="37" t="s">
+      <c r="A21" s="35" t="s">
         <v>87</v>
       </c>
+      <c r="B21" s="99" t="s">
+        <v>107</v>
+      </c>
       <c r="C21" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+        <v>113</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="39"/>
+        <v>98</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="37"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="34" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="37"/>
+        <v>98</v>
+      </c>
+      <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="34" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>90</v>
+      <c r="C25" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="34" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>90</v>
+        <v>100</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>90</v>
+        <v>100</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="34" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>90</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D28" s="35"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="34" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="34" t="s">
         <v>64</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="34" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>52</v>
+      <c r="A33" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="99" t="s">
+        <v>110</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>52</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>90</v>
+        <v>103</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="31" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>45</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>90</v>
+        <v>104</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>73</v>
+        <v>36</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>73</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>55</v>
+        <v>77</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>76</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B40" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>90</v>
+      <c r="C40" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3302,7 +3353,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C13" sqref="C13:I13"/>
+      <selection pane="topRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3327,23 +3378,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="53" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="41" t="s">
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="67" t="s">
+      <c r="K1" s="41"/>
+      <c r="L1" s="66" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -3384,7 +3435,7 @@
       <c r="K2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="68"/>
+      <c r="L2" s="67"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
@@ -3414,11 +3465,11 @@
         <v>28</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="44" t="str">
+      <c r="C4" s="43" t="str">
         <f>'Drug Information'!$B5</f>
         <v>Flucloxacillin</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3435,12 +3486,12 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="44" t="str">
+      <c r="D5" s="43" t="str">
         <f>'Drug Information'!$B7</f>
         <v>Amoxicillin</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -3457,14 +3508,14 @@
         <v>30</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="47" t="str">
+      <c r="C6" s="46" t="str">
         <f>'Drug Information'!$B11</f>
         <v>Cefazolin</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -3477,14 +3528,14 @@
         <v>31</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="47" t="str">
+      <c r="C7" s="46" t="str">
         <f>'Drug Information'!$B15</f>
         <v>Cefoxitin</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="49"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -3496,40 +3547,40 @@
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="47" t="str">
+      <c r="C8" s="46" t="str">
         <f>'Drug Information'!$B17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="49"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="47" t="str">
+      <c r="I8" s="46" t="str">
         <f>'Drug Information'!$B17</f>
         <v>Ceftriaxone</v>
       </c>
-      <c r="J8" s="62"/>
-      <c r="K8" s="49"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="48"/>
       <c r="L8" s="6"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="47" t="str">
+      <c r="D9" s="46" t="str">
         <f>'Drug Information'!$B18</f>
         <v>Ceftazidime</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="49"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -3541,34 +3592,34 @@
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="63" t="str">
+      <c r="C10" s="62" t="str">
         <f>'Drug Information'!$B19</f>
         <v>Cefepime</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="49"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="48"/>
       <c r="L10" s="6"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="50" t="str">
+      <c r="C11" s="49" t="str">
         <f>'Drug Information'!$B8</f>
         <v>Amoxicillin-Clavulanic Acid</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -3580,86 +3631,86 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="50" t="str">
+      <c r="C12" s="49" t="str">
         <f>'Drug Information'!$B9</f>
-        <v>Ampicillin/Sulbactam</v>
-      </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
+        <v>Ampicillin-Sulbactam</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="11" t="str">
         <f>'Drug Information'!$B9</f>
-        <v>Ampicillin/Sulbactam</v>
+        <v>Ampicillin-Sulbactam</v>
       </c>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="65" t="str">
+      <c r="C13" s="64" t="str">
         <f>'Drug Information'!$B10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="66"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="65"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="65" t="str">
+      <c r="K13" s="64" t="str">
         <f>'Drug Information'!$B10</f>
         <v>Piperacillin-Tazobactam</v>
       </c>
-      <c r="L13" s="66"/>
+      <c r="L13" s="65"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="76" t="str">
+      <c r="C14" s="75" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="78"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="76" t="str">
+      <c r="I14" s="75" t="str">
         <f>'Drug Information'!$B22</f>
         <v>Ertapenem</v>
       </c>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="78"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="77"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="76" t="str">
+      <c r="C15" s="75" t="str">
         <f>'Drug Information'!$B24</f>
         <v>Meropenem</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="78"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="77"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3669,20 +3720,20 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="79" t="s">
+      <c r="E16" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="81"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="80"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
@@ -3691,34 +3742,34 @@
         <v>Ciprofloxacin</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="85" t="str">
+      <c r="E17" s="84" t="str">
         <f>'Drug Information'!$B26</f>
         <v>Ciprofloxacin</v>
       </c>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="87"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="86"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="85" t="str">
+      <c r="C18" s="84" t="str">
         <f>'Drug Information'!$B27</f>
         <v>Levofloxacin</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="89"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="88"/>
       <c r="L18" s="6"/>
       <c r="M18" s="12" t="str">
         <f>'Drug Information'!$B27</f>
@@ -3726,25 +3777,25 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="59" t="str">
+      <c r="C19" s="58" t="str">
         <f>'Drug Information'!$B28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="61"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="59" t="str">
+      <c r="I19" s="58" t="str">
         <f>'Drug Information'!$B28</f>
         <v>Moxifloxacin</v>
       </c>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="61"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="60"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -3753,14 +3804,14 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="92" t="str">
+      <c r="E20" s="91" t="str">
         <f>'Drug Information'!$B31</f>
         <v>Amikacin</v>
       </c>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="95"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="94"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -3770,12 +3821,12 @@
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="69" t="str">
-        <f>'Drug Information'!$B33</f>
+      <c r="B21" s="68" t="str">
+        <f>'Drug Information'!$B34</f>
         <v>Clindamycin</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="71"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3784,7 +3835,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="13" t="str">
-        <f>'Drug Information'!$B33</f>
+        <f>'Drug Information'!$B34</f>
         <v>Clindamycin</v>
       </c>
       <c r="M21" s="14"/>
@@ -3794,11 +3845,11 @@
         <v>17</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="90" t="str">
+      <c r="C22" s="89" t="str">
         <f>'Drug Information'!$B32</f>
         <v>Azithromycin</v>
       </c>
-      <c r="D22" s="91"/>
+      <c r="D22" s="90"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3819,25 +3870,25 @@
       <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="96" t="str">
-        <f>'Drug Information'!$B34</f>
+      <c r="B23" s="95" t="str">
+        <f>'Drug Information'!$B35</f>
         <v>Doxycycline</v>
       </c>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="98"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="97"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="17" t="str">
-        <f>'Drug Information'!$B34</f>
+        <f>'Drug Information'!$B35</f>
         <v>Doxycycline</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="17" t="str">
-        <f>'Drug Information'!$B34</f>
+        <f>'Drug Information'!$B35</f>
         <v>Doxycycline</v>
       </c>
     </row>
@@ -3845,12 +3896,12 @@
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="72" t="str">
-        <f>'Drug Information'!$B35</f>
+      <c r="B24" s="71" t="str">
+        <f>'Drug Information'!$B36</f>
         <v>Vancomycin</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="74"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="73"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3865,15 +3916,15 @@
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="82" t="str">
-        <f>'Drug Information'!$B38</f>
+      <c r="B25" s="81" t="str">
+        <f>'Drug Information'!$B39</f>
         <v>Trimethoprim/Sulfamethoxazole</v>
       </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="84"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="83"/>
       <c r="H25" s="6"/>
       <c r="I25" s="18" t="s">
         <v>18</v>
@@ -3900,27 +3951,27 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="20" t="str">
-        <f>'Drug Information'!$B39</f>
+        <f>'Drug Information'!$B40</f>
         <v>Metronidazole</v>
       </c>
       <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>